<commit_message>
Added Stauber and Jeffrey 1988
</commit_message>
<xml_diff>
--- a/aux/pigment_distribution.xlsx
+++ b/aux/pigment_distribution.xlsx
@@ -81,6 +81,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Reported in Lauridsen et al. (2006). Small values of Cantha and Echin found in one strain of DIATO_1 (</t>
     </r>
     <r>
@@ -535,10 +542,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -735,17 +742,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -759,59 +766,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -826,7 +781,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -848,6 +818,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -856,11 +833,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -885,7 +892,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -897,13 +964,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,91 +1048,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,49 +1060,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1245,7 +1252,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1261,24 +1268,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1323,126 +1312,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1451,16 +1458,16 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2278,9 +2285,9 @@
   <dimension ref="A1:AT58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B$1:C$1048576"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Added Brotas and Plante-Cuny 2003
</commit_message>
<xml_diff>
--- a/aux/pigment_distribution.xlsx
+++ b/aux/pigment_distribution.xlsx
@@ -542,10 +542,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -742,17 +742,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,6 +787,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -781,7 +826,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -789,14 +834,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -811,36 +857,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -848,24 +864,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -886,6 +886,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -898,55 +994,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -958,61 +1024,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,43 +1060,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1233,17 +1233,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1252,7 +1246,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1268,6 +1262,47 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1289,185 +1324,150 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2285,9 +2285,9 @@
   <dimension ref="A1:AT58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P$1:P$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2305,7 +2305,8 @@
     <col min="33" max="35" width="4.625" style="10" customWidth="1"/>
     <col min="36" max="36" width="4.625" style="9" customWidth="1"/>
     <col min="37" max="37" width="4.625" style="10" customWidth="1"/>
-    <col min="38" max="45" width="4.625" style="9" customWidth="1"/>
+    <col min="38" max="38" width="3.75" style="9" customWidth="1"/>
+    <col min="39" max="45" width="4.625" style="9" customWidth="1"/>
     <col min="46" max="46" width="4.625" style="10" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>